<commit_message>
added data + RHEO parse script
</commit_message>
<xml_diff>
--- a/jupyter/RHEO/flow curv.xlsx
+++ b/jupyter/RHEO/flow curv.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729503AA-8C68-4E77-905B-5F508D0DFEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01C70D3-FC78-4C6F-854B-D1D8629708DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="19188" windowHeight="11448" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLA" sheetId="1" r:id="rId1"/>
@@ -1824,7 +1824,7 @@
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="A1:XFD1048576"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3259,7 +3259,7 @@
   <dimension ref="A1:P103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="A1:XFD1048576"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6013,7 +6013,7 @@
   <dimension ref="A1:P103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>